<commit_message>
Tests for all valid templates and fixes to corresponding importers.
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Experiment_run_Infinium_v5_3_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Experiment_run_Infinium_v5_3_0.xlsx
@@ -2222,7 +2222,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO996"/>
+  <dimension ref="A1:AO997"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -2702,169 +2702,166 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="16"/>
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+      <c r="AK7" s="16"/>
+      <c r="AL7" s="16"/>
+      <c r="AM7" s="16"/>
+      <c r="AN7" s="16"/>
+      <c r="AO7" s="16"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="3" t="str">
-        <f aca="false">IF(B7&lt;&gt;"", B7, "")</f>
-        <v>hh</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="R7" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA7" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK7" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO7" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="B8" s="3"/>
       <c r="C8" s="3" t="str">
         <f aca="false">IF(B8&lt;&gt;"", B8, "")</f>
-        <v/>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+        <v>hh</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
+      <c r="P8" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
+      <c r="U8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA8" s="17" t="s">
+        <v>78</v>
+      </c>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
+      <c r="AC8" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL8" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="AM8" s="3"/>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="3"/>
+      <c r="AN8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO8" s="18" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17"/>
@@ -3234,7 +3231,7 @@
       <c r="AN16" s="3"/>
       <c r="AO16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="str">
@@ -7101,7 +7098,10 @@
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="17"/>
       <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
+      <c r="C101" s="3" t="str">
+        <f aca="false">IF(B101&lt;&gt;"", B101, "")</f>
+        <v/>
+      </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
@@ -16215,7 +16215,7 @@
       <c r="AO312" s="3"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A313" s="3"/>
+      <c r="A313" s="17"/>
       <c r="B313" s="3"/>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -45626,22 +45626,65 @@
       <c r="AN996" s="3"/>
       <c r="AO996" s="3"/>
     </row>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A997" s="3"/>
+      <c r="B997" s="3"/>
+      <c r="C997" s="3"/>
+      <c r="D997" s="3"/>
+      <c r="E997" s="3"/>
+      <c r="F997" s="3"/>
+      <c r="G997" s="3"/>
+      <c r="H997" s="3"/>
+      <c r="I997" s="3"/>
+      <c r="J997" s="3"/>
+      <c r="K997" s="3"/>
+      <c r="L997" s="3"/>
+      <c r="M997" s="3"/>
+      <c r="N997" s="3"/>
+      <c r="O997" s="3"/>
+      <c r="P997" s="3"/>
+      <c r="Q997" s="3"/>
+      <c r="R997" s="3"/>
+      <c r="S997" s="3"/>
+      <c r="T997" s="3"/>
+      <c r="U997" s="3"/>
+      <c r="V997" s="3"/>
+      <c r="W997" s="3"/>
+      <c r="X997" s="3"/>
+      <c r="Y997" s="3"/>
+      <c r="Z997" s="3"/>
+      <c r="AA997" s="3"/>
+      <c r="AB997" s="3"/>
+      <c r="AC997" s="3"/>
+      <c r="AD997" s="3"/>
+      <c r="AE997" s="3"/>
+      <c r="AF997" s="3"/>
+      <c r="AG997" s="3"/>
+      <c r="AH997" s="3"/>
+      <c r="AI997" s="3"/>
+      <c r="AJ997" s="3"/>
+      <c r="AK997" s="3"/>
+      <c r="AL997" s="3"/>
+      <c r="AM997" s="3"/>
+      <c r="AN997" s="3"/>
+      <c r="AO997" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C7:C100">
+  <conditionalFormatting sqref="C8:C101">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>SUMPRODUCT(--ISNUMBER(SEARCH(MID(C7, ROW(INDIRECT("1:" &amp; LEN(C7))), 1), "ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz0123456789-_")))&lt;&gt;LEN(C7)</formula>
+      <formula>SUMPRODUCT(--ISNUMBER(SEARCH(MID(C8, ROW(INDIRECT("1:" &amp; LEN(C8))), 1), "ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz0123456789-_")))&lt;&gt;LEN(C8)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D100" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D8:D101" type="list">
       <formula1>Index!$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E100" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E8:E101" type="list">
       <formula1>Index!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="A7:A312" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="A8:A313" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -45662,7 +45705,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -45750,37 +45793,38 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="23"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="F6" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -45902,27 +45946,27 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="24"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="23"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="23"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -46727,7 +46771,10 @@
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
-      <c r="F101" s="3"/>
+      <c r="E101" s="23"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3"/>
@@ -53022,37 +53069,44 @@
       <c r="D1000" s="3"/>
       <c r="F1000" s="3"/>
     </row>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1001" s="3"/>
+      <c r="B1001" s="3"/>
+      <c r="C1001" s="3"/>
+      <c r="D1001" s="3"/>
+      <c r="F1001" s="3"/>
+    </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G100 F101" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G101 F102" type="list">
       <formula1>Index!$D$2:$D$25</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
-      <formula1>Experiments!$A$7:$A$106</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A6:A101" type="list">
+      <formula1>Experiments!$A$8:$A$107</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5:H100" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H101" type="none">
       <formula1>Index!$D$2:$D$25</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5:I100" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I101" type="list">
       <formula1>Index!$G$2:$G$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E100" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E101" type="none">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G5:G8 G10:G99" type="list">
-      <formula1>INDIRECT(SUBSTITUTE(INDEX(Experiments!$E$7:$E$173, MATCH($A5,Experiments!$A$7:$A$173,0))," ","_"))</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G9 G11:G100" type="list">
+      <formula1>INDIRECT(SUBSTITUTE(INDEX(Experiments!$E$8:$E$174, MATCH($A5,Experiments!$A$8:$A$174,0))," ","_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G9" type="list">
-      <formula1>INDIRECT(SUBSTITUTE(INDEX(Experiments!$E$7:$E$100, MATCH($A9,Experiments!$A$7:$A$100,0))," ","_"))</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G10" type="list">
+      <formula1>INDIRECT(SUBSTITUTE(INDEX(Experiments!$E$8:$E$101, MATCH($A10,Experiments!$A$8:$A$101,0))," ","_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D102" type="none">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>